<commit_message>
itt van az összes jelenlegi ip-cím amit beleraktam, minden feltüntetve
</commit_message>
<xml_diff>
--- a/vizsgaremek_vlsm.xlsx
+++ b/vizsgaremek_vlsm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\vizsgaremekHM\Vizsgaremek_2025_firstteam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076F4518-99EA-4F4F-A670-02FC2453ABC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BEC231F-2325-46E6-8E90-E55A35E111E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{49EBFCAF-62DE-4318-9C36-661E52DD0866}"/>
+    <workbookView xWindow="3390" yWindow="6285" windowWidth="21600" windowHeight="11385" xr2:uid="{49EBFCAF-62DE-4318-9C36-661E52DD0866}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Publikus IP-címek az ISP felé</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Router interfész (ISP felé)</t>
   </si>
   <si>
-    <t>Publikus IP</t>
-  </si>
-  <si>
     <t>203.0.113.2/30</t>
   </si>
   <si>
@@ -59,15 +56,6 @@
     <t>203.0.113.10/30</t>
   </si>
   <si>
-    <t>G0/2 → ISP_R Fa0/1/2</t>
-  </si>
-  <si>
-    <t>G0/2 → ISP_R Fa0/1/1</t>
-  </si>
-  <si>
-    <t>G0/1 → ISP_R Fa0/1/0</t>
-  </si>
-  <si>
     <t>4-esével növekszik</t>
   </si>
   <si>
@@ -83,7 +71,88 @@
     <t>Debrecen - R3</t>
   </si>
   <si>
-    <t>Távmunkás környezet</t>
+    <t>WAN - 1.1.1.0 255.255.255.0/24</t>
+  </si>
+  <si>
+    <t>Távmunkás környezet - NAT</t>
+  </si>
+  <si>
+    <t>Privát IP-k a telephelyeken (titkárságok egy másik közeli épületben)</t>
+  </si>
+  <si>
+    <t>Hálózat</t>
+  </si>
+  <si>
+    <t>Router IP</t>
+  </si>
+  <si>
+    <t>Budapest (központ)</t>
+  </si>
+  <si>
+    <t>192.168.10.0/24</t>
+  </si>
+  <si>
+    <t>192.168.10.1</t>
+  </si>
+  <si>
+    <t>Debrecen</t>
+  </si>
+  <si>
+    <t>192.168.20.0/24</t>
+  </si>
+  <si>
+    <t>192.168.20.1</t>
+  </si>
+  <si>
+    <t>Szeged</t>
+  </si>
+  <si>
+    <t>192.168.30.0/24</t>
+  </si>
+  <si>
+    <t>192.168.30.1</t>
+  </si>
+  <si>
+    <t>Budapest titkárság</t>
+  </si>
+  <si>
+    <t>192.168.11.0/24</t>
+  </si>
+  <si>
+    <t>192.168.11.1</t>
+  </si>
+  <si>
+    <t>192.168.31.0/24</t>
+  </si>
+  <si>
+    <t>Szeged titkárság</t>
+  </si>
+  <si>
+    <t>192.168.31.1</t>
+  </si>
+  <si>
+    <t>LAN - 192.168.50.0 255.255.255.0/24 vlan 20-ban működik</t>
+  </si>
+  <si>
+    <t>G0/2 → ISP_R G0/1</t>
+  </si>
+  <si>
+    <t>G0/2 → ISP_R G0/2</t>
+  </si>
+  <si>
+    <t>Távmunkás SOHO</t>
+  </si>
+  <si>
+    <t>ROUTER_INTERFACE → ISP_R G0/0</t>
+  </si>
+  <si>
+    <t>1.1.1.1/24</t>
+  </si>
+  <si>
+    <t>Gig0/0/0(optikai kábel itt) → Gig0/2/0</t>
+  </si>
+  <si>
+    <t>Publikus IP (Routeré, az isp routeren 1-el kisebb szám)</t>
   </si>
 </sst>
 </file>
@@ -114,12 +183,18 @@
       <name val="Arial Unicode MS"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -134,16 +209,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -479,82 +558,173 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EEC1A7D-5AEA-4B02-8190-D1FD3F0A5485}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="60">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="45">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="45">
+      <c r="A6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:3" ht="30">
+      <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="60">
-      <c r="A2" s="1" t="s">
+    </row>
+    <row r="9" spans="1:3" ht="45">
+      <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="45">
+      <c r="A11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="30">
-      <c r="A3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="30">
-      <c r="A4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="30">
-      <c r="A5" s="2" t="s">
+      <c r="B12" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="2" t="s">
+      <c r="C12" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vlanok és acl-ek beleirva
</commit_message>
<xml_diff>
--- a/vizsgaremek_vlsm.xlsx
+++ b/vizsgaremek_vlsm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\vizsgaremekHM\Vizsgaremek_2025_firstteam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BEC231F-2325-46E6-8E90-E55A35E111E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2413B5D0-8020-4803-8931-F2719D1F69BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3390" yWindow="6285" windowWidth="21600" windowHeight="11385" xr2:uid="{49EBFCAF-62DE-4318-9C36-661E52DD0866}"/>
+    <workbookView xWindow="8625" yWindow="1305" windowWidth="21600" windowHeight="11385" xr2:uid="{49EBFCAF-62DE-4318-9C36-661E52DD0866}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t>Publikus IP-címek az ISP felé</t>
   </si>
@@ -153,6 +153,48 @@
   </si>
   <si>
     <t>Publikus IP (Routeré, az isp routeren 1-el kisebb szám)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vlanok </t>
+  </si>
+  <si>
+    <t>SALES</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>MARKETING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vlan 110 </t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>vlan 120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vlan 130 </t>
+  </si>
+  <si>
+    <t>MANAGEMENT (native)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vlan 99 </t>
+  </si>
+  <si>
+    <t>ACL_BUDAPESTEN</t>
+  </si>
+  <si>
+    <t>access-list 1 permit 192.168.110.0 0.0.0.255</t>
+  </si>
+  <si>
+    <t>access-list 1 permit 192.168.120.0 0.0.0.255</t>
+  </si>
+  <si>
+    <t>access-list 1 permit 192.168.130.0 0.0.0.255</t>
   </si>
 </sst>
 </file>
@@ -183,7 +225,7 @@
       <name val="Arial Unicode MS"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -193,6 +235,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -209,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -223,6 +271,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -558,15 +610,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EEC1A7D-5AEA-4B02-8190-D1FD3F0A5485}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -638,93 +690,166 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:3" ht="30">
-      <c r="A8" s="1" t="s">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:3" ht="30">
+      <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="45">
-      <c r="A9" s="1" t="s">
+    <row r="11" spans="1:3" ht="45">
+      <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="45">
-      <c r="A11" s="3" t="s">
+    <row r="13" spans="1:3" ht="45">
+      <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
         <v>29</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B19" t="s">
         <v>28</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C19" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="6"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dns szerver már működik
</commit_message>
<xml_diff>
--- a/vizsgaremek_vlsm.xlsx
+++ b/vizsgaremek_vlsm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\vizsgaremekHM\Vizsgaremek_2025_firstteam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2413B5D0-8020-4803-8931-F2719D1F69BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05AC665E-AB1D-4C7D-8056-1EF923084AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8625" yWindow="1305" windowWidth="21600" windowHeight="11385" xr2:uid="{49EBFCAF-62DE-4318-9C36-661E52DD0866}"/>
+    <workbookView xWindow="5280" yWindow="2520" windowWidth="21600" windowHeight="11385" xr2:uid="{49EBFCAF-62DE-4318-9C36-661E52DD0866}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
   <si>
     <t>Publikus IP-címek az ISP felé</t>
   </si>
@@ -62,15 +62,6 @@
     <t>kábelkötések</t>
   </si>
   <si>
-    <t>Budapest - R1</t>
-  </si>
-  <si>
-    <t>Szeged - R2</t>
-  </si>
-  <si>
-    <t>Debrecen - R3</t>
-  </si>
-  <si>
     <t>WAN - 1.1.1.0 255.255.255.0/24</t>
   </si>
   <si>
@@ -89,12 +80,6 @@
     <t>Budapest (központ)</t>
   </si>
   <si>
-    <t>192.168.10.0/24</t>
-  </si>
-  <si>
-    <t>192.168.10.1</t>
-  </si>
-  <si>
     <t>Debrecen</t>
   </si>
   <si>
@@ -155,9 +140,6 @@
     <t>Publikus IP (Routeré, az isp routeren 1-el kisebb szám)</t>
   </si>
   <si>
-    <t xml:space="preserve">Vlanok </t>
-  </si>
-  <si>
     <t>SALES</t>
   </si>
   <si>
@@ -185,9 +167,6 @@
     <t xml:space="preserve">vlan 99 </t>
   </si>
   <si>
-    <t>ACL_BUDAPESTEN</t>
-  </si>
-  <si>
     <t>access-list 1 permit 192.168.110.0 0.0.0.255</t>
   </si>
   <si>
@@ -195,13 +174,70 @@
   </si>
   <si>
     <t>access-list 1 permit 192.168.130.0 0.0.0.255</t>
+  </si>
+  <si>
+    <t>DNS-HTTP kiszolgálás, céges webserver</t>
+  </si>
+  <si>
+    <t>192.168.99.50</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>192.168.110.0/24</t>
+  </si>
+  <si>
+    <t>192.168.120.0/24</t>
+  </si>
+  <si>
+    <t>192.168.130.0/24</t>
+  </si>
+  <si>
+    <t>192.168.99.0/24</t>
+  </si>
+  <si>
+    <t>access-list 1 permit 192.168.99.0 0.0.0.255</t>
+  </si>
+  <si>
+    <t>Budapest BP_R</t>
+  </si>
+  <si>
+    <t>Szeged - SZEG_R</t>
+  </si>
+  <si>
+    <t>Debrecen - DEB_R</t>
+  </si>
+  <si>
+    <t>VLANOK - 110.0 , 120.0 , 130.0 , 99.0</t>
+  </si>
+  <si>
+    <t>192.168.99.1</t>
+  </si>
+  <si>
+    <t>Vlanok BUDAPEST</t>
+  </si>
+  <si>
+    <t>ACL BUDAPEST</t>
+  </si>
+  <si>
+    <t>SERVEREK BUDAPEST</t>
+  </si>
+  <si>
+    <t>Távmunkás szimulációs példa</t>
+  </si>
+  <si>
+    <t>192.168.50.0/24</t>
+  </si>
+  <si>
+    <t>192.168.50.1/24</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,6 +259,21 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -257,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -265,16 +316,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -612,45 +664,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EEC1A7D-5AEA-4B02-8190-D1FD3F0A5485}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="60">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>38</v>
+      <c r="C2" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
@@ -658,10 +710,10 @@
     </row>
     <row r="4" spans="1:3" ht="30">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>4</v>
@@ -669,190 +721,226 @@
     </row>
     <row r="5" spans="1:3" ht="45">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="45">
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="2"/>
+      <c r="A7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="3" t="s">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30">
+      <c r="A9" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30">
+      <c r="A10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" ht="30">
-      <c r="A10" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="45">
-      <c r="A11" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="45">
-      <c r="A13" s="3" t="s">
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" t="s">
-        <v>27</v>
+      <c r="A18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="6"/>
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="C22" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" t="s">
-        <v>45</v>
-      </c>
+      <c r="A23" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
+      <c r="A26" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>51</v>
-      </c>
+      <c r="A28" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>46</v>
+      </c>
+      <c r="B29" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
dns már működik, vlanok jók, mindenki eléri a szolgáltatót
</commit_message>
<xml_diff>
--- a/vizsgaremek_vlsm.xlsx
+++ b/vizsgaremek_vlsm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\vizsgaremekHM\Vizsgaremek_2025_firstteam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05AC665E-AB1D-4C7D-8056-1EF923084AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D407577-9504-4AA9-8C3E-12C84792FF00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5280" yWindow="2520" windowWidth="21600" windowHeight="11385" xr2:uid="{49EBFCAF-62DE-4318-9C36-661E52DD0866}"/>
   </bookViews>
@@ -664,8 +664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EEC1A7D-5AEA-4B02-8190-D1FD3F0A5485}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>